<commit_message>
Cambio modelo de Hoja A3
organizo hoja de esquematico a formato A3. Incluyo libreria de conector UFL. Organizo Alimentacion, incluyo bobinas para I/O salidas. Incluyo switches de EN y de Programacion IO0, IO2, incluyo algunos condensadores y leds
</commit_message>
<xml_diff>
--- a/Info/ESP32 Pins.xlsx
+++ b/Info/ESP32 Pins.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\poved\OneDrive - Blackstone\Maestria\Semestre I\Fabricacion SE\Microcontrolador\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\poved\OneDrive - Blackstone\Maestria\Semestre I\Fabricacion SE\SE_Datalog\Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="38640" windowHeight="21240"/>
+    <workbookView xWindow="1740" yWindow="-120" windowWidth="38640" windowHeight="21240"/>
   </bookViews>
   <sheets>
     <sheet name="WROOM" sheetId="2" r:id="rId1"/>
@@ -253,7 +253,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="330">
   <si>
     <t>ADC</t>
   </si>
@@ -1241,6 +1241,9 @@
   </si>
   <si>
     <t>BOOT OPTION</t>
+  </si>
+  <si>
+    <t>ENTRADAS</t>
   </si>
 </sst>
 </file>
@@ -1310,7 +1313,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1359,6 +1362,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1372,7 +1381,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1404,6 +1413,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1728,7 +1739,7 @@
   <dimension ref="A1:V43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2424,7 +2435,7 @@
       <c r="A18" s="3">
         <v>27</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="24" t="s">
         <v>41</v>
       </c>
       <c r="C18" s="20" t="s">
@@ -2453,7 +2464,7 @@
       <c r="A19" s="3">
         <v>28</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="24" t="s">
         <v>43</v>
       </c>
       <c r="C19" s="20" t="s">
@@ -2737,7 +2748,7 @@
       <c r="A30" s="3">
         <v>6</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="23" t="s">
         <v>9</v>
       </c>
       <c r="C30" s="4" t="s">
@@ -2772,7 +2783,7 @@
       <c r="A31" s="3">
         <v>7</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="23" t="s">
         <v>10</v>
       </c>
       <c r="C31" s="4" t="s">
@@ -2807,7 +2818,7 @@
       <c r="A32" s="3">
         <v>4</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="23" t="s">
         <v>7</v>
       </c>
       <c r="C32" s="4" t="s">
@@ -2842,7 +2853,7 @@
       <c r="A33" s="3">
         <v>5</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="23" t="s">
         <v>8</v>
       </c>
       <c r="C33" s="4" t="s">
@@ -2911,6 +2922,10 @@
       <c r="T41" s="6"/>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B42" s="23"/>
+      <c r="C42" s="14" t="s">
+        <v>329</v>
+      </c>
       <c r="G42" s="8"/>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
@@ -2933,7 +2948,7 @@
   <dimension ref="A1:L86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A29" sqref="A29:H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3100,7 +3115,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -3138,7 +3153,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>212</v>
       </c>
@@ -3176,7 +3191,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>213</v>
       </c>
@@ -3214,7 +3229,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -3252,7 +3267,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>214</v>
       </c>
@@ -3287,7 +3302,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>215</v>
       </c>
@@ -3325,7 +3340,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>216</v>
       </c>
@@ -4567,7 +4582,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>228</v>
       </c>
@@ -4602,7 +4617,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>230</v>
       </c>
@@ -4672,7 +4687,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>231</v>
       </c>
@@ -4707,7 +4722,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>207</v>
       </c>
@@ -4961,7 +4976,9 @@
   <autoFilter ref="A1:L86">
     <filterColumn colId="2">
       <filters>
+        <filter val="I"/>
         <filter val="I/O"/>
+        <filter val="O"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>